<commit_message>
SSDM-13256: Added Registration Date, Registrator, Modification Date and Modifier export support for experiments.
</commit_message>
<xml_diff>
--- a/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-experiment.xlsx
+++ b/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-experiment.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
   <si>
     <t xml:space="preserve">EXPERIMENT</t>
   </si>
@@ -40,6 +40,18 @@
     <t xml:space="preserve">Project</t>
   </si>
   <si>
+    <t xml:space="preserve">Registrator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registration Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modifier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modification Date</t>
+  </si>
+  <si>
     <t xml:space="preserve">Name</t>
   </si>
   <si>
@@ -53,6 +65,18 @@
   </si>
   <si>
     <t xml:space="preserve">/ELN_SETTINGS/STORAGES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-03-10 17:23:44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023-03-11 17:23:44</t>
   </si>
   <si>
     <t xml:space="preserve">EXPERIMENTAL_STEP</t>
@@ -95,9 +119,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -202,44 +227,52 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -256,146 +289,228 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ12"/>
+  <dimension ref="A1:AMJ13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5:D6"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="34.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="8.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="34.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="1022" style="1" width="8.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
+      <c r="B2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" s="7" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="H4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="3" t="s">
+      <c r="I4" s="6" t="s">
         <v>11</v>
       </c>
+    </row>
+    <row r="5" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="8"/>
+      <c r="I5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AMH5" s="1"/>
+      <c r="AMI5" s="0"/>
       <c r="AMJ5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="3" t="s">
+      <c r="A6" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>15</v>
       </c>
+      <c r="E6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" s="8"/>
+      <c r="I6" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="4"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" s="9" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AMH11" s="1"/>
+      <c r="AMI11" s="0"/>
+      <c r="AMJ11" s="0"/>
+    </row>
+    <row r="12" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" s="7" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="5" t="s">
+      <c r="F12" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="AMJ11" s="0"/>
-    </row>
-    <row r="12" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
+      <c r="G12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>22</v>
-      </c>
+      <c r="H12" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E13" s="7"/>
+      <c r="F13" s="0"/>
+      <c r="G13" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
SSDM-13256: Added missing column for experiment.
</commit_message>
<xml_diff>
--- a/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-experiment.xlsx
+++ b/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-experiment.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="35">
   <si>
     <t xml:space="preserve">EXPERIMENT</t>
   </si>
@@ -31,6 +31,9 @@
     <t xml:space="preserve">COLLECTION</t>
   </si>
   <si>
+    <t xml:space="preserve">PermId</t>
+  </si>
+  <si>
     <t xml:space="preserve">Identifier</t>
   </si>
   <si>
@@ -58,6 +61,9 @@
     <t xml:space="preserve">Default object type</t>
   </si>
   <si>
+    <t xml:space="preserve">200001010000000-0001</t>
+  </si>
+  <si>
     <t xml:space="preserve">/ELN_SETTINGS/STORAGES/STORAGES_COLLECTION</t>
   </si>
   <si>
@@ -82,6 +88,9 @@
     <t xml:space="preserve">EXPERIMENTAL_STEP</t>
   </si>
   <si>
+    <t xml:space="preserve">200001010000000-0003</t>
+  </si>
+  <si>
     <t xml:space="preserve">/TEST/TEST/TEST</t>
   </si>
   <si>
@@ -98,6 +107,9 @@
   </si>
   <si>
     <t xml:space="preserve">Experiment completed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200001010000000-0002</t>
   </si>
   <si>
     <t xml:space="preserve">/DEFAULT/DEFAULT/DEFAULT</t>
@@ -293,10 +305,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ13"/>
+  <dimension ref="A1:XFC13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -304,13 +316,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="34.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="18.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="20.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1022" min="1022" style="1" width="8.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="0" width="8.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16383" style="1" width="8.37"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -334,10 +346,10 @@
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -352,73 +364,87 @@
       <c r="G4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="J4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="AMH4" s="0"/>
+      <c r="AMI4" s="1"/>
+      <c r="XFC4" s="0"/>
     </row>
     <row r="5" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>12</v>
+      <c r="A5" s="0" t="s">
+        <v>13</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="D5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="E5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="F5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="8"/>
-      <c r="I5" s="4" t="s">
+      <c r="G5" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AMH5" s="1"/>
-      <c r="AMI5" s="0"/>
-      <c r="AMJ5" s="0"/>
+      <c r="H5" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="8"/>
+      <c r="J5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="AMI5" s="1"/>
+      <c r="AMJ5" s="1"/>
+      <c r="AMK5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H6" s="8"/>
-      <c r="I6" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="I6" s="8"/>
+      <c r="J6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AMH6" s="0"/>
+      <c r="AMI6" s="1"/>
+      <c r="XFC6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
@@ -426,7 +452,6 @@
       </c>
       <c r="B8" s="4"/>
       <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
@@ -435,25 +460,23 @@
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
     </row>
     <row r="11" s="9" customFormat="true" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -468,48 +491,56 @@
       <c r="G11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="AMH11" s="1"/>
-      <c r="AMI11" s="0"/>
-      <c r="AMJ11" s="0"/>
+      <c r="I11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AMI11" s="1"/>
+      <c r="AMJ11" s="1"/>
+      <c r="AMK11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="0" t="s">
+      <c r="A12" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="F12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>30</v>
-      </c>
+      <c r="G12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="AMH12" s="0"/>
+      <c r="AMI12" s="1"/>
+      <c r="XFC12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E13" s="7"/>
-      <c r="F13" s="0"/>
       <c r="G13" s="7"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BIS-790: Working on exporting too large cell data as external files. Fixed the corresponding XLS export tests.
</commit_message>
<xml_diff>
--- a/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-experiment.xlsx
+++ b/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-experiment.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="37">
   <si>
     <t xml:space="preserve">EXPERIMENT</t>
   </si>
@@ -85,6 +85,9 @@
     <t xml:space="preserve">2023-03-11 17:23:44</t>
   </si>
   <si>
+    <t xml:space="preserve">__value-I5.txt__</t>
+  </si>
+  <si>
     <t xml:space="preserve">EXPERIMENTAL_STEP</t>
   </si>
   <si>
@@ -98,6 +101,9 @@
   </si>
   <si>
     <t xml:space="preserve">/TEST/TEST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">__value-I6.txt__</t>
   </si>
   <si>
     <t xml:space="preserve">DEFAULT_SAMPLE</t>
@@ -191,18 +197,12 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF993300"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -272,7 +272,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -300,18 +300,124 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:XFC13"/>
+  <dimension ref="A1:AMK13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.52734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="34.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.83"/>
@@ -373,12 +479,10 @@
       <c r="J4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="AMH4" s="0"/>
       <c r="AMI4" s="1"/>
-      <c r="XFC4" s="0"/>
     </row>
     <row r="5" s="9" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -402,26 +506,28 @@
       <c r="H5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I5" s="8"/>
+      <c r="I5" s="8" t="s">
+        <v>21</v>
+      </c>
       <c r="J5" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AMI5" s="1"/>
       <c r="AMJ5" s="1"/>
       <c r="AMK5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>22</v>
+      <c r="A6" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>17</v>
@@ -435,13 +541,13 @@
       <c r="H6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I6" s="8"/>
+      <c r="I6" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="J6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="AMH6" s="0"/>
+        <v>28</v>
+      </c>
       <c r="AMI6" s="1"/>
-      <c r="XFC6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H7" s="1"/>
@@ -463,7 +569,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -498,24 +604,24 @@
         <v>11</v>
       </c>
       <c r="J11" s="6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="AMI11" s="1"/>
       <c r="AMJ11" s="1"/>
       <c r="AMK11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>29</v>
+      <c r="A12" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>17</v>
@@ -530,14 +636,12 @@
         <v>20</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J12" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="AMH12" s="0"/>
+        <v>36</v>
+      </c>
       <c r="AMI12" s="1"/>
-      <c r="XFC12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E13" s="7"/>

</xml_diff>